<commit_message>
add BC_MH to batch 3
</commit_message>
<xml_diff>
--- a/curation/BC_Package_2023_03_31.xlsx
+++ b/curation/BC_Package_2023_03_31.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_github\cdisc-org\COSMoS\curation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E3F5CC6-64B2-4295-9C56-2F88A60DBA38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BCB0C3E-8B9F-4C73-BBED-E82FA2954BDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="7" xr2:uid="{FA29263D-F7AA-4D0C-AE9B-6B008D3B18BE}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13096" activeTab="5" xr2:uid="{FA29263D-F7AA-4D0C-AE9B-6B008D3B18BE}"/>
   </bookViews>
   <sheets>
     <sheet name="BC_DM" sheetId="27" r:id="rId1"/>
@@ -18,16 +18,17 @@
     <sheet name="BC_LB" sheetId="8" r:id="rId3"/>
     <sheet name="BC_MB" sheetId="28" r:id="rId4"/>
     <sheet name="BC_AE" sheetId="36" r:id="rId5"/>
-    <sheet name="BC_CM" sheetId="33" r:id="rId6"/>
-    <sheet name="BC_RE" sheetId="30" r:id="rId7"/>
-    <sheet name="BC_PR" sheetId="31" r:id="rId8"/>
-    <sheet name="BC_BE" sheetId="29" r:id="rId9"/>
-    <sheet name="BC_EG" sheetId="22" r:id="rId10"/>
-    <sheet name="BC_DS" sheetId="14" r:id="rId11"/>
-    <sheet name="NCIt Placeholders" sheetId="13" r:id="rId12"/>
+    <sheet name="BC_MH" sheetId="37" r:id="rId6"/>
+    <sheet name="BC_CM" sheetId="33" r:id="rId7"/>
+    <sheet name="BC_RE" sheetId="30" r:id="rId8"/>
+    <sheet name="BC_PR" sheetId="31" r:id="rId9"/>
+    <sheet name="BC_BE" sheetId="29" r:id="rId10"/>
+    <sheet name="BC_EG" sheetId="22" r:id="rId11"/>
+    <sheet name="BC_DS" sheetId="14" r:id="rId12"/>
+    <sheet name="NCIt Placeholders" sheetId="13" r:id="rId13"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">BC_EG!$A$1:$O$73</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">BC_EG!$A$1:$O$73</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">BC_LB!$A$1:$P$67</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">BC_VS!$A$1:$O$8</definedName>
   </definedNames>
@@ -52,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2362" uniqueCount="520">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2440" uniqueCount="536">
   <si>
     <t>package_date</t>
   </si>
@@ -1626,6 +1627,54 @@
   </si>
   <si>
     <t>A radiographic procedure using the emission of x-rays to form an image of the structure penetrated by the radiation.</t>
+  </si>
+  <si>
+    <t>The collected name for an event observation.</t>
+  </si>
+  <si>
+    <t>Reported Events; Medical History Events; Medical Conditions; Presenting Conditions</t>
+  </si>
+  <si>
+    <t>C83118</t>
+  </si>
+  <si>
+    <t>Medical History Reported Term</t>
+  </si>
+  <si>
+    <t>Medical History; MHTERM</t>
+  </si>
+  <si>
+    <t>C83346</t>
+  </si>
+  <si>
+    <t>Medical History Dictionary Derived Term</t>
+  </si>
+  <si>
+    <t>C83018</t>
+  </si>
+  <si>
+    <t>Medical History Category</t>
+  </si>
+  <si>
+    <t>C83143</t>
+  </si>
+  <si>
+    <t>Medical History Subcategory</t>
+  </si>
+  <si>
+    <t>C87897</t>
+  </si>
+  <si>
+    <t>Medical History Pre-specified</t>
+  </si>
+  <si>
+    <t>C83067</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Medical History Occurrence </t>
+  </si>
+  <si>
+    <t>The verbatim description of the medical history being reported.</t>
   </si>
 </sst>
 </file>
@@ -2348,23 +2397,23 @@
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="47.5703125" customWidth="1"/>
+    <col min="2" max="2" width="47.59765625" customWidth="1"/>
     <col min="4" max="4" width="6" customWidth="1"/>
-    <col min="5" max="5" width="25.7109375" customWidth="1"/>
-    <col min="6" max="6" width="19.28515625" style="9" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.73046875" customWidth="1"/>
+    <col min="6" max="6" width="19.265625" style="9" customWidth="1"/>
+    <col min="7" max="7" width="10.73046875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="72" style="9" customWidth="1"/>
-    <col min="9" max="9" width="7.140625" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="7.1328125" hidden="1" customWidth="1"/>
     <col min="10" max="10" width="6" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="5.140625" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="27.7109375" customWidth="1"/>
-    <col min="15" max="15" width="49.85546875" customWidth="1"/>
+    <col min="11" max="11" width="5.1328125" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="27.73046875" customWidth="1"/>
+    <col min="15" max="15" width="49.86328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" s="1" customFormat="1" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
@@ -2411,7 +2460,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A2" s="19" t="s">
         <v>15</v>
       </c>
@@ -2435,7 +2484,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A3" s="19" t="s">
         <v>15</v>
       </c>
@@ -2459,7 +2508,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A4" s="19" t="s">
         <v>15</v>
       </c>
@@ -2486,7 +2535,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A5" s="19" t="s">
         <v>15</v>
       </c>
@@ -2506,7 +2555,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A6" s="19" t="s">
         <v>15</v>
       </c>
@@ -2532,7 +2581,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A7" s="19" t="s">
         <v>15</v>
       </c>
@@ -2555,7 +2604,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A8" s="19" t="s">
         <v>15</v>
       </c>
@@ -2581,7 +2630,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="90" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A9" s="19" t="s">
         <v>15</v>
       </c>
@@ -2604,7 +2653,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A10" s="19" t="s">
         <v>15</v>
       </c>
@@ -2656,6 +2705,297 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DC7AE7F-1668-415E-8316-B69305094CC9}">
+  <dimension ref="A1:P9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O5" sqref="O5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.3984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.59765625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="50" customWidth="1"/>
+    <col min="9" max="9" width="6.3984375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="4.73046875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20" customWidth="1"/>
+    <col min="15" max="15" width="10.73046875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" s="41" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A1" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="41" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="41" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="41" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="41" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="41" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="42" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="41" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="41" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="41" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="41" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="41" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="41" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="42" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A2" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
+        <v>339</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>340</v>
+      </c>
+      <c r="D2" s="39"/>
+      <c r="E2" s="37" t="s">
+        <v>341</v>
+      </c>
+      <c r="F2" t="s">
+        <v>342</v>
+      </c>
+      <c r="G2" s="37" t="s">
+        <v>32</v>
+      </c>
+      <c r="H2" s="38" t="s">
+        <v>343</v>
+      </c>
+      <c r="I2" s="100"/>
+      <c r="J2" s="100"/>
+      <c r="K2" s="100"/>
+      <c r="L2" s="100"/>
+      <c r="M2" s="37"/>
+      <c r="N2" s="37"/>
+      <c r="O2" s="37"/>
+      <c r="P2" s="37"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A3" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
+        <v>339</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>340</v>
+      </c>
+      <c r="D3" s="39"/>
+      <c r="E3" s="37" t="s">
+        <v>344</v>
+      </c>
+      <c r="G3" s="37"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="100"/>
+      <c r="J3" s="100"/>
+      <c r="K3" s="37"/>
+      <c r="L3" s="15" t="s">
+        <v>345</v>
+      </c>
+      <c r="M3" s="37" t="s">
+        <v>346</v>
+      </c>
+      <c r="N3" s="37" t="s">
+        <v>27</v>
+      </c>
+      <c r="O3" s="37"/>
+      <c r="P3" s="37"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A4" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>339</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>340</v>
+      </c>
+      <c r="D4" s="39"/>
+      <c r="E4" s="37" t="s">
+        <v>344</v>
+      </c>
+      <c r="G4" s="37"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="100"/>
+      <c r="J4" s="100"/>
+      <c r="K4" s="37"/>
+      <c r="L4" s="15" t="s">
+        <v>347</v>
+      </c>
+      <c r="M4" s="37" t="s">
+        <v>348</v>
+      </c>
+      <c r="N4" s="37" t="s">
+        <v>27</v>
+      </c>
+      <c r="O4" s="37" t="s">
+        <v>516</v>
+      </c>
+      <c r="P4" s="37"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A5" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
+        <v>339</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>340</v>
+      </c>
+      <c r="D5" s="39"/>
+      <c r="E5" s="37" t="s">
+        <v>344</v>
+      </c>
+      <c r="G5" s="37"/>
+      <c r="H5" s="38"/>
+      <c r="I5" s="100"/>
+      <c r="J5" s="100"/>
+      <c r="K5" s="37"/>
+      <c r="L5" s="15" t="s">
+        <v>349</v>
+      </c>
+      <c r="M5" s="37" t="s">
+        <v>350</v>
+      </c>
+      <c r="N5" s="37" t="s">
+        <v>27</v>
+      </c>
+      <c r="O5" s="37"/>
+      <c r="P5" s="37"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A6" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>339</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>340</v>
+      </c>
+      <c r="D6" s="39"/>
+      <c r="E6" s="37" t="s">
+        <v>344</v>
+      </c>
+      <c r="G6" s="37"/>
+      <c r="H6" s="38"/>
+      <c r="I6" s="100"/>
+      <c r="J6" s="100"/>
+      <c r="K6" s="37"/>
+      <c r="L6" s="15" t="s">
+        <v>351</v>
+      </c>
+      <c r="M6" s="37" t="s">
+        <v>352</v>
+      </c>
+      <c r="N6" s="37" t="s">
+        <v>27</v>
+      </c>
+      <c r="O6" s="37"/>
+      <c r="P6" s="37"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A7" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
+        <v>339</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>340</v>
+      </c>
+      <c r="D7" s="15"/>
+      <c r="E7" s="37" t="s">
+        <v>344</v>
+      </c>
+      <c r="H7" s="9"/>
+      <c r="L7" s="15" t="s">
+        <v>353</v>
+      </c>
+      <c r="M7" s="37" t="s">
+        <v>354</v>
+      </c>
+      <c r="N7" s="37" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A8" s="40"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="H8" s="9"/>
+      <c r="L8" s="15"/>
+      <c r="M8" s="37"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A9" s="40"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="H9" s="9"/>
+      <c r="L9" s="15"/>
+      <c r="M9" s="37"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="I5:J5"/>
+  </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="L3" r:id="rId1" display="https://ncithesaurus.nci.nih.gov/ncitbrowser/ConceptReport.jsp?dictionary=NCI_Thesaurus&amp;ns=ncit&amp;code=C82571" xr:uid="{4F336F55-DA38-4BFA-A8FE-1B50799B12D9}"/>
+    <hyperlink ref="L4" r:id="rId2" display="https://evsexplore.nci.nih.gov/evsexplore/concept/ncit/C82977" xr:uid="{84616E4F-44BE-4656-94FE-3CAEDF7CDCB9}"/>
+    <hyperlink ref="L5" r:id="rId3" display="https://ncithesaurus.nci.nih.gov/ncitbrowser/ConceptReport.jsp?dictionary=NCI_Thesaurus&amp;ns=ncit&amp;code=C25372" xr:uid="{7D202BF9-76BC-40DB-9E31-E3CC4E640E24}"/>
+    <hyperlink ref="L6" r:id="rId4" display="https://ncithesaurus.nci.nih.gov/ncitbrowser/ConceptReport.jsp?dictionary=NCI_Thesaurus&amp;ns=ncit&amp;code=C25692" xr:uid="{089EDE5B-41FF-4CA6-878A-1C77F1E5873E}"/>
+    <hyperlink ref="C2" r:id="rId5" xr:uid="{8CA55E9B-8F6C-4EFA-BFDA-4D26710188D6}"/>
+    <hyperlink ref="C3:C6" r:id="rId6" display="C70945" xr:uid="{3EAC77A3-7633-4967-9FE5-4584FEB6951E}"/>
+    <hyperlink ref="L7" r:id="rId7" xr:uid="{3A80CB5A-691C-4326-A475-9708183012A1}"/>
+    <hyperlink ref="C7" r:id="rId8" xr:uid="{1C9D9F76-9433-40B0-AF2A-78150A167C1E}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FA66AC2-B345-487D-8D73-AE011EF2E448}">
   <dimension ref="A1:O107"/>
   <sheetViews>
@@ -2663,21 +3003,21 @@
       <selection activeCell="O80" sqref="O80"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.1328125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25" customWidth="1"/>
-    <col min="4" max="4" width="8.140625" customWidth="1"/>
-    <col min="5" max="5" width="38.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="32.7109375" customWidth="1"/>
-    <col min="7" max="7" width="11.5703125" customWidth="1"/>
-    <col min="8" max="8" width="56.28515625" customWidth="1"/>
-    <col min="13" max="13" width="31.85546875" customWidth="1"/>
+    <col min="4" max="4" width="8.1328125" customWidth="1"/>
+    <col min="5" max="5" width="38.265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="32.73046875" customWidth="1"/>
+    <col min="7" max="7" width="11.59765625" customWidth="1"/>
+    <col min="8" max="8" width="56.265625" customWidth="1"/>
+    <col min="13" max="13" width="31.86328125" customWidth="1"/>
     <col min="15" max="15" width="65" customWidth="1"/>
     <col min="16" max="16" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
@@ -2724,7 +3064,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15" s="43" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" s="43" customFormat="1" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A2" s="80" t="s">
         <v>15</v>
       </c>
@@ -2746,7 +3086,7 @@
       </c>
       <c r="L2" s="51"/>
     </row>
-    <row r="3" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A3" s="14" t="s">
         <v>15</v>
       </c>
@@ -2785,7 +3125,7 @@
       <c r="N3" s="12"/>
       <c r="O3" s="12"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A4" s="14" t="s">
         <v>15</v>
       </c>
@@ -2820,7 +3160,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A5" s="14" t="s">
         <v>15</v>
       </c>
@@ -2855,7 +3195,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A6" s="14" t="s">
         <v>15</v>
       </c>
@@ -2890,7 +3230,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A7" s="14" t="s">
         <v>15</v>
       </c>
@@ -2925,7 +3265,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A8" s="14" t="s">
         <v>15</v>
       </c>
@@ -2960,7 +3300,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A9" s="14" t="s">
         <v>15</v>
       </c>
@@ -2995,7 +3335,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="10" spans="1:15" s="43" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" s="43" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A10" s="80" t="s">
         <v>15</v>
       </c>
@@ -3017,7 +3357,7 @@
       </c>
       <c r="L10" s="51"/>
     </row>
-    <row r="11" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" ht="57" x14ac:dyDescent="0.45">
       <c r="A11" s="14" t="s">
         <v>15</v>
       </c>
@@ -3053,7 +3393,7 @@
       </c>
       <c r="L11" s="4"/>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A12" s="14" t="s">
         <v>15</v>
       </c>
@@ -3088,7 +3428,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A13" s="14" t="s">
         <v>15</v>
       </c>
@@ -3123,7 +3463,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A14" s="14" t="s">
         <v>15</v>
       </c>
@@ -3152,7 +3492,7 @@
       </c>
       <c r="O14" s="12"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A15" s="14" t="s">
         <v>15</v>
       </c>
@@ -3183,7 +3523,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A16" s="14" t="s">
         <v>15</v>
       </c>
@@ -3216,7 +3556,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A17" s="14" t="s">
         <v>15</v>
       </c>
@@ -3247,7 +3587,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="18" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A18" s="14" t="s">
         <v>15</v>
       </c>
@@ -3283,7 +3623,7 @@
       </c>
       <c r="L18" s="4"/>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A19" s="14" t="s">
         <v>15</v>
       </c>
@@ -3318,7 +3658,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A20" s="14" t="s">
         <v>15</v>
       </c>
@@ -3353,7 +3693,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A21" s="14" t="s">
         <v>15</v>
       </c>
@@ -3382,7 +3722,7 @@
       </c>
       <c r="O21" s="12"/>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A22" s="14" t="s">
         <v>15</v>
       </c>
@@ -3413,7 +3753,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A23" s="14" t="s">
         <v>15</v>
       </c>
@@ -3446,7 +3786,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A24" s="14" t="s">
         <v>15</v>
       </c>
@@ -3477,7 +3817,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="25" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A25" s="14" t="s">
         <v>15</v>
       </c>
@@ -3513,7 +3853,7 @@
       </c>
       <c r="L25" s="4"/>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A26" s="14" t="s">
         <v>15</v>
       </c>
@@ -3548,7 +3888,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A27" s="14" t="s">
         <v>15</v>
       </c>
@@ -3583,7 +3923,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A28" s="14" t="s">
         <v>15</v>
       </c>
@@ -3612,7 +3952,7 @@
       </c>
       <c r="O28" s="12"/>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A29" s="14" t="s">
         <v>15</v>
       </c>
@@ -3643,7 +3983,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A30" s="14" t="s">
         <v>15</v>
       </c>
@@ -3676,7 +4016,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A31" s="14" t="s">
         <v>15</v>
       </c>
@@ -3707,7 +4047,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="32" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A32" s="14" t="s">
         <v>15</v>
       </c>
@@ -3743,7 +4083,7 @@
       </c>
       <c r="L32" s="4"/>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A33" s="14" t="s">
         <v>15</v>
       </c>
@@ -3778,7 +4118,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A34" s="14" t="s">
         <v>15</v>
       </c>
@@ -3813,7 +4153,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A35" s="14" t="s">
         <v>15</v>
       </c>
@@ -3842,7 +4182,7 @@
       </c>
       <c r="O35" s="12"/>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A36" s="14" t="s">
         <v>15</v>
       </c>
@@ -3873,7 +4213,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A37" s="14" t="s">
         <v>15</v>
       </c>
@@ -3906,7 +4246,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A38" s="14" t="s">
         <v>15</v>
       </c>
@@ -3937,7 +4277,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="39" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15" ht="57" x14ac:dyDescent="0.45">
       <c r="A39" s="14" t="s">
         <v>15</v>
       </c>
@@ -3973,7 +4313,7 @@
       </c>
       <c r="L39" s="4"/>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A40" s="14" t="s">
         <v>15</v>
       </c>
@@ -4008,7 +4348,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A41" s="14" t="s">
         <v>15</v>
       </c>
@@ -4043,7 +4383,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A42" s="14" t="s">
         <v>15</v>
       </c>
@@ -4076,7 +4416,7 @@
       </c>
       <c r="O42" s="12"/>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A43" s="14" t="s">
         <v>15</v>
       </c>
@@ -4111,7 +4451,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A44" s="14" t="s">
         <v>15</v>
       </c>
@@ -4144,7 +4484,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A45" s="14" t="s">
         <v>15</v>
       </c>
@@ -4175,7 +4515,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="46" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:15" ht="57" x14ac:dyDescent="0.45">
       <c r="A46" s="14" t="s">
         <v>15</v>
       </c>
@@ -4211,7 +4551,7 @@
       </c>
       <c r="L46" s="4"/>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A47" s="14" t="s">
         <v>15</v>
       </c>
@@ -4246,7 +4586,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A48" s="14" t="s">
         <v>15</v>
       </c>
@@ -4281,7 +4621,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A49" s="14" t="s">
         <v>15</v>
       </c>
@@ -4314,7 +4654,7 @@
       </c>
       <c r="O49" s="12"/>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A50" s="14" t="s">
         <v>15</v>
       </c>
@@ -4349,7 +4689,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A51" s="14" t="s">
         <v>15</v>
       </c>
@@ -4382,7 +4722,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A52" s="14" t="s">
         <v>15</v>
       </c>
@@ -4413,7 +4753,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="53" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:15" ht="57" x14ac:dyDescent="0.45">
       <c r="A53" s="14" t="s">
         <v>15</v>
       </c>
@@ -4449,7 +4789,7 @@
       </c>
       <c r="L53" s="4"/>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A54" s="14" t="s">
         <v>15</v>
       </c>
@@ -4484,7 +4824,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A55" s="14" t="s">
         <v>15</v>
       </c>
@@ -4519,7 +4859,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A56" s="14" t="s">
         <v>15</v>
       </c>
@@ -4552,7 +4892,7 @@
       </c>
       <c r="O56" s="12"/>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A57" s="14" t="s">
         <v>15</v>
       </c>
@@ -4587,7 +4927,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A58" s="14" t="s">
         <v>15</v>
       </c>
@@ -4620,7 +4960,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A59" s="14" t="s">
         <v>15</v>
       </c>
@@ -4651,7 +4991,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="60" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:15" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A60" s="14" t="s">
         <v>15</v>
       </c>
@@ -4685,7 +5025,7 @@
       </c>
       <c r="L60" s="4"/>
     </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A61" s="14" t="s">
         <v>15</v>
       </c>
@@ -4720,7 +5060,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A62" s="14" t="s">
         <v>15</v>
       </c>
@@ -4755,7 +5095,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A63" s="14" t="s">
         <v>15</v>
       </c>
@@ -4788,7 +5128,7 @@
       </c>
       <c r="O63" s="12"/>
     </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A64" s="14" t="s">
         <v>15</v>
       </c>
@@ -4823,7 +5163,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A65" s="14" t="s">
         <v>15</v>
       </c>
@@ -4856,7 +5196,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A66" s="14" t="s">
         <v>15</v>
       </c>
@@ -4887,7 +5227,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="67" spans="1:15" ht="75" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:15" ht="57" x14ac:dyDescent="0.45">
       <c r="A67" s="14" t="s">
         <v>15</v>
       </c>
@@ -4923,7 +5263,7 @@
       </c>
       <c r="L67" s="4"/>
     </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A68" s="14" t="s">
         <v>15</v>
       </c>
@@ -4958,7 +5298,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A69" s="14" t="s">
         <v>15</v>
       </c>
@@ -4993,7 +5333,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A70" s="14" t="s">
         <v>15</v>
       </c>
@@ -5026,7 +5366,7 @@
       </c>
       <c r="O70" s="12"/>
     </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A71" s="14" t="s">
         <v>15</v>
       </c>
@@ -5061,7 +5401,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A72" s="14" t="s">
         <v>15</v>
       </c>
@@ -5094,7 +5434,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A73" s="14" t="s">
         <v>15</v>
       </c>
@@ -5125,7 +5465,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A74" s="14"/>
       <c r="C74" s="4"/>
       <c r="D74" s="4"/>
@@ -5133,7 +5473,7 @@
       <c r="H74" s="9"/>
       <c r="L74" s="4"/>
     </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A75" s="14"/>
       <c r="C75" s="4"/>
       <c r="D75" s="4"/>
@@ -5141,7 +5481,7 @@
       <c r="H75" s="9"/>
       <c r="L75" s="4"/>
     </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A76" s="14"/>
       <c r="C76" s="4"/>
       <c r="D76" s="4"/>
@@ -5149,7 +5489,7 @@
       <c r="H76" s="9"/>
       <c r="L76" s="4"/>
     </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A77" s="14"/>
       <c r="C77" s="4"/>
       <c r="D77" s="4"/>
@@ -5157,7 +5497,7 @@
       <c r="H77" s="9"/>
       <c r="L77" s="4"/>
     </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A78" s="14"/>
       <c r="C78" s="4"/>
       <c r="D78" s="4"/>
@@ -5165,7 +5505,7 @@
       <c r="H78" s="9"/>
       <c r="L78" s="4"/>
     </row>
-    <row r="79" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A79" s="14"/>
       <c r="C79" s="4"/>
       <c r="D79" s="4"/>
@@ -5173,7 +5513,7 @@
       <c r="H79" s="9"/>
       <c r="L79" s="4"/>
     </row>
-    <row r="80" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A80" s="14"/>
       <c r="C80" s="4"/>
       <c r="D80" s="4"/>
@@ -5181,7 +5521,7 @@
       <c r="H80" s="9"/>
       <c r="L80" s="4"/>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A81" s="14"/>
       <c r="C81" s="4"/>
       <c r="D81" s="4"/>
@@ -5189,7 +5529,7 @@
       <c r="H81" s="9"/>
       <c r="L81" s="4"/>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A82" s="14"/>
       <c r="C82" s="4"/>
       <c r="D82" s="4"/>
@@ -5197,7 +5537,7 @@
       <c r="H82" s="9"/>
       <c r="L82" s="4"/>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A83" s="14"/>
       <c r="C83" s="4"/>
       <c r="D83" s="4"/>
@@ -5205,7 +5545,7 @@
       <c r="H83" s="9"/>
       <c r="L83" s="4"/>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A84" s="14"/>
       <c r="C84" s="4"/>
       <c r="D84" s="4"/>
@@ -5213,7 +5553,7 @@
       <c r="H84" s="9"/>
       <c r="L84" s="4"/>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A85" s="14"/>
       <c r="C85" s="4"/>
       <c r="D85" s="4"/>
@@ -5221,7 +5561,7 @@
       <c r="H85" s="9"/>
       <c r="L85" s="4"/>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A86" s="14"/>
       <c r="C86" s="4"/>
       <c r="D86" s="4"/>
@@ -5229,7 +5569,7 @@
       <c r="H86" s="9"/>
       <c r="L86" s="4"/>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A87" s="14"/>
       <c r="C87" s="4"/>
       <c r="D87" s="4"/>
@@ -5237,7 +5577,7 @@
       <c r="H87" s="9"/>
       <c r="L87" s="4"/>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A88" s="14"/>
       <c r="C88" s="4"/>
       <c r="D88" s="4"/>
@@ -5245,7 +5585,7 @@
       <c r="H88" s="9"/>
       <c r="L88" s="4"/>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A89" s="14"/>
       <c r="C89" s="4"/>
       <c r="D89" s="4"/>
@@ -5253,7 +5593,7 @@
       <c r="H89" s="9"/>
       <c r="L89" s="4"/>
     </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A90" s="14"/>
       <c r="C90" s="4"/>
       <c r="D90" s="4"/>
@@ -5261,7 +5601,7 @@
       <c r="H90" s="9"/>
       <c r="L90" s="4"/>
     </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A91" s="14"/>
       <c r="C91" s="4"/>
       <c r="D91" s="4"/>
@@ -5269,7 +5609,7 @@
       <c r="H91" s="9"/>
       <c r="L91" s="4"/>
     </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A92" s="14"/>
       <c r="C92" s="4"/>
       <c r="D92" s="4"/>
@@ -5277,7 +5617,7 @@
       <c r="H92" s="9"/>
       <c r="L92" s="4"/>
     </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A93" s="14"/>
       <c r="C93" s="4"/>
       <c r="D93" s="4"/>
@@ -5285,7 +5625,7 @@
       <c r="H93" s="9"/>
       <c r="L93" s="4"/>
     </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A94" s="14"/>
       <c r="C94" s="4"/>
       <c r="D94" s="4"/>
@@ -5293,7 +5633,7 @@
       <c r="H94" s="9"/>
       <c r="L94" s="4"/>
     </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A95" s="14"/>
       <c r="C95" s="4"/>
       <c r="D95" s="4"/>
@@ -5301,7 +5641,7 @@
       <c r="H95" s="9"/>
       <c r="L95" s="4"/>
     </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A96" s="14"/>
       <c r="C96" s="4"/>
       <c r="D96" s="4"/>
@@ -5309,7 +5649,7 @@
       <c r="H96" s="9"/>
       <c r="L96" s="4"/>
     </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A97" s="14"/>
       <c r="C97" s="4"/>
       <c r="D97" s="4"/>
@@ -5317,7 +5657,7 @@
       <c r="H97" s="9"/>
       <c r="L97" s="4"/>
     </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A98" s="14"/>
       <c r="C98" s="4"/>
       <c r="D98" s="4"/>
@@ -5325,7 +5665,7 @@
       <c r="H98" s="9"/>
       <c r="L98" s="4"/>
     </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A99" s="14"/>
       <c r="C99" s="4"/>
       <c r="D99" s="4"/>
@@ -5333,7 +5673,7 @@
       <c r="H99" s="9"/>
       <c r="L99" s="4"/>
     </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A100" s="14"/>
       <c r="C100" s="4"/>
       <c r="D100" s="4"/>
@@ -5341,7 +5681,7 @@
       <c r="H100" s="9"/>
       <c r="L100" s="4"/>
     </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A101" s="14"/>
       <c r="C101" s="4"/>
       <c r="D101" s="4"/>
@@ -5349,7 +5689,7 @@
       <c r="H101" s="9"/>
       <c r="L101" s="4"/>
     </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A102" s="14"/>
       <c r="C102" s="4"/>
       <c r="D102" s="4"/>
@@ -5357,7 +5697,7 @@
       <c r="H102" s="9"/>
       <c r="L102" s="4"/>
     </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A103" s="14"/>
       <c r="C103" s="4"/>
       <c r="D103" s="4"/>
@@ -5365,7 +5705,7 @@
       <c r="H103" s="9"/>
       <c r="L103" s="4"/>
     </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A104" s="14"/>
       <c r="C104" s="4"/>
       <c r="D104" s="4"/>
@@ -5373,7 +5713,7 @@
       <c r="H104" s="9"/>
       <c r="L104" s="4"/>
     </row>
-    <row r="105" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A105" s="14"/>
       <c r="C105" s="4"/>
       <c r="D105" s="4"/>
@@ -5381,7 +5721,7 @@
       <c r="H105" s="9"/>
       <c r="L105" s="4"/>
     </row>
-    <row r="106" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A106" s="14"/>
       <c r="C106" s="4"/>
       <c r="D106" s="4"/>
@@ -5389,7 +5729,7 @@
       <c r="H106" s="9"/>
       <c r="L106" s="4"/>
     </row>
-    <row r="107" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A107" s="14"/>
       <c r="C107" s="4"/>
       <c r="D107" s="4"/>
@@ -5508,7 +5848,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2110127A-6DB5-413E-8873-1BEF9F2EE846}">
   <dimension ref="A1:O33"/>
   <sheetViews>
@@ -5516,24 +5856,24 @@
       <selection activeCell="O32" sqref="O32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="12" style="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.7109375" style="14" customWidth="1"/>
-    <col min="4" max="4" width="9.28515625" customWidth="1"/>
-    <col min="5" max="5" width="46.7109375" customWidth="1"/>
-    <col min="6" max="6" width="24.140625" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" customWidth="1"/>
-    <col min="8" max="8" width="68.28515625" style="9" customWidth="1"/>
-    <col min="9" max="9" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.42578125" customWidth="1"/>
-    <col min="11" max="11" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.73046875" style="14" customWidth="1"/>
+    <col min="4" max="4" width="9.265625" customWidth="1"/>
+    <col min="5" max="5" width="46.73046875" customWidth="1"/>
+    <col min="6" max="6" width="24.1328125" customWidth="1"/>
+    <col min="7" max="7" width="11.3984375" customWidth="1"/>
+    <col min="8" max="8" width="68.265625" style="9" customWidth="1"/>
+    <col min="9" max="9" width="6.3984375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.3984375" customWidth="1"/>
+    <col min="11" max="11" width="4.73046875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="32" customWidth="1"/>
-    <col min="14" max="14" width="13.140625" customWidth="1"/>
-    <col min="15" max="15" width="31.85546875" customWidth="1"/>
+    <col min="14" max="14" width="13.1328125" customWidth="1"/>
+    <col min="15" max="15" width="31.86328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5580,7 +5920,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15" s="43" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" s="43" customFormat="1" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A2" s="80" t="s">
         <v>15</v>
       </c>
@@ -5599,7 +5939,7 @@
       </c>
       <c r="L2" s="50"/>
     </row>
-    <row r="3" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A3" s="14" t="s">
         <v>15</v>
       </c>
@@ -5625,7 +5965,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A4" s="14" t="s">
         <v>15</v>
       </c>
@@ -5652,7 +5992,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A5" s="14" t="s">
         <v>15</v>
       </c>
@@ -5682,7 +6022,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A6" s="14" t="s">
         <v>15</v>
       </c>
@@ -5709,7 +6049,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A7" s="14" t="s">
         <v>15</v>
       </c>
@@ -5736,7 +6076,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A8" s="14" t="s">
         <v>15</v>
       </c>
@@ -5762,7 +6102,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A9" s="14" t="s">
         <v>15</v>
       </c>
@@ -5788,7 +6128,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A10" s="14" t="s">
         <v>15</v>
       </c>
@@ -5817,7 +6157,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A11" s="14" t="s">
         <v>15</v>
       </c>
@@ -5843,7 +6183,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A12" s="14" t="s">
         <v>15</v>
       </c>
@@ -5869,7 +6209,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A13" s="14" t="s">
         <v>15</v>
       </c>
@@ -5895,7 +6235,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A14" s="14" t="s">
         <v>15</v>
       </c>
@@ -5921,7 +6261,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A15" s="14" t="s">
         <v>15</v>
       </c>
@@ -5950,7 +6290,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A16" s="14" t="s">
         <v>15</v>
       </c>
@@ -5976,7 +6316,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A17" s="14" t="s">
         <v>15</v>
       </c>
@@ -6002,7 +6342,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:15" s="43" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" s="43" customFormat="1" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A18" s="43" t="s">
         <v>15</v>
       </c>
@@ -6023,7 +6363,7 @@
       </c>
       <c r="L18" s="50"/>
     </row>
-    <row r="19" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A19" s="14" t="s">
         <v>15</v>
       </c>
@@ -6049,7 +6389,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A20" s="14" t="s">
         <v>15</v>
       </c>
@@ -6075,7 +6415,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A21" s="14" t="s">
         <v>15</v>
       </c>
@@ -6104,7 +6444,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A22" s="14" t="s">
         <v>15</v>
       </c>
@@ -6130,7 +6470,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A23" s="14" t="s">
         <v>15</v>
       </c>
@@ -6156,7 +6496,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="24" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A24" s="14" t="s">
         <v>15</v>
       </c>
@@ -6179,7 +6519,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A25" s="14" t="s">
         <v>15</v>
       </c>
@@ -6205,7 +6545,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A26" s="14" t="s">
         <v>15</v>
       </c>
@@ -6234,7 +6574,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A27" s="14" t="s">
         <v>15</v>
       </c>
@@ -6260,7 +6600,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A28" s="14" t="s">
         <v>15</v>
       </c>
@@ -6286,7 +6626,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A29" s="14" t="s">
         <v>15</v>
       </c>
@@ -6309,7 +6649,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A30" s="14" t="s">
         <v>15</v>
       </c>
@@ -6335,7 +6675,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A31" s="14" t="s">
         <v>15</v>
       </c>
@@ -6364,7 +6704,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A32" s="14" t="s">
         <v>15</v>
       </c>
@@ -6390,7 +6730,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A33" s="14" t="s">
         <v>15</v>
       </c>
@@ -6477,7 +6817,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6253F1A8-4D53-4FEC-828B-55F619DE8B8E}">
   <dimension ref="A1:C10"/>
   <sheetViews>
@@ -6485,16 +6825,16 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="99" customWidth="1"/>
-    <col min="3" max="3" width="62.28515625" customWidth="1"/>
-    <col min="4" max="4" width="19.42578125" customWidth="1"/>
-    <col min="5" max="5" width="55.85546875" customWidth="1"/>
+    <col min="3" max="3" width="62.265625" customWidth="1"/>
+    <col min="4" max="4" width="19.3984375" customWidth="1"/>
+    <col min="5" max="5" width="55.86328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>485</v>
       </c>
@@ -6502,7 +6842,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="72" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" s="72" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A2" s="56" t="s">
         <v>487</v>
       </c>
@@ -6513,7 +6853,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="56" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" s="56" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A3" s="56" t="s">
         <v>87</v>
       </c>
@@ -6521,7 +6861,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="56" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" s="56" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A4" s="56" t="s">
         <v>490</v>
       </c>
@@ -6529,7 +6869,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="56" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" s="56" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A5" s="56" t="s">
         <v>179</v>
       </c>
@@ -6537,7 +6877,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6" s="56" t="s">
         <v>176</v>
       </c>
@@ -6545,7 +6885,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>491</v>
       </c>
@@ -6556,7 +6896,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>491</v>
       </c>
@@ -6581,22 +6921,22 @@
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="14.140625" style="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="49.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.7109375" customWidth="1"/>
+    <col min="1" max="1" width="14.1328125" style="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49.86328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.73046875" customWidth="1"/>
     <col min="5" max="5" width="27" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.5703125" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="85.85546875" customWidth="1"/>
-    <col min="9" max="9" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.59765625" customWidth="1"/>
+    <col min="7" max="7" width="10.73046875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="85.86328125" customWidth="1"/>
+    <col min="9" max="9" width="13.86328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.3984375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.1328125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="109" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" s="1" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
@@ -6643,7 +6983,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="43" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" s="43" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A2" s="91" t="s">
         <v>15</v>
       </c>
@@ -6674,7 +7014,7 @@
       <c r="P2" s="67"/>
       <c r="Q2" s="67"/>
     </row>
-    <row r="3" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A3" s="14" t="s">
         <v>15</v>
       </c>
@@ -6711,7 +7051,7 @@
       <c r="L3" s="64"/>
       <c r="Q3" s="65"/>
     </row>
-    <row r="4" spans="1:17" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" ht="15.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="14" t="s">
         <v>15</v>
       </c>
@@ -6738,7 +7078,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A5" s="14" t="s">
         <v>15</v>
       </c>
@@ -6768,7 +7108,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A6" s="14" t="s">
         <v>15</v>
       </c>
@@ -6797,7 +7137,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A7" s="14" t="s">
         <v>15</v>
       </c>
@@ -6826,7 +7166,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A8" s="14" t="s">
         <v>15</v>
       </c>
@@ -6887,28 +7227,28 @@
       <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" style="19" customWidth="1"/>
+    <col min="1" max="1" width="10.265625" style="19" customWidth="1"/>
     <col min="2" max="2" width="68" style="2" customWidth="1"/>
-    <col min="3" max="3" width="11.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="47.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" style="7" customWidth="1"/>
-    <col min="7" max="7" width="13.7109375" style="2" customWidth="1"/>
-    <col min="8" max="8" width="57.28515625" style="3" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" style="3" customWidth="1"/>
-    <col min="10" max="10" width="8.5703125" style="3" customWidth="1"/>
-    <col min="11" max="11" width="7.5703125" style="2" customWidth="1"/>
-    <col min="12" max="12" width="11.140625" style="2" customWidth="1"/>
-    <col min="13" max="13" width="31.28515625" style="2" customWidth="1"/>
-    <col min="14" max="14" width="9.7109375" style="2" customWidth="1"/>
-    <col min="15" max="15" width="23.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="29.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.73046875" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="47.86328125" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.73046875" style="7" customWidth="1"/>
+    <col min="7" max="7" width="13.73046875" style="2" customWidth="1"/>
+    <col min="8" max="8" width="57.265625" style="3" customWidth="1"/>
+    <col min="9" max="9" width="10.73046875" style="3" customWidth="1"/>
+    <col min="10" max="10" width="8.59765625" style="3" customWidth="1"/>
+    <col min="11" max="11" width="7.59765625" style="2" customWidth="1"/>
+    <col min="12" max="12" width="11.1328125" style="2" customWidth="1"/>
+    <col min="13" max="13" width="31.265625" style="2" customWidth="1"/>
+    <col min="14" max="14" width="9.73046875" style="2" customWidth="1"/>
+    <col min="15" max="15" width="23.265625" style="3" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="29.265625" style="2" bestFit="1" customWidth="1"/>
     <col min="17" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="26" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" s="26" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A1" s="30" t="s">
         <v>0</v>
       </c>
@@ -6958,7 +7298,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" ht="15.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="19" t="s">
         <v>15</v>
       </c>
@@ -6986,7 +7326,7 @@
       <c r="I2" s="17"/>
       <c r="J2" s="10"/>
     </row>
-    <row r="3" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A3" s="19" t="s">
         <v>15</v>
       </c>
@@ -7014,7 +7354,7 @@
       </c>
       <c r="O3" s="10"/>
     </row>
-    <row r="4" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A4" s="19" t="s">
         <v>15</v>
       </c>
@@ -7042,7 +7382,7 @@
       </c>
       <c r="O4" s="10"/>
     </row>
-    <row r="5" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A5" s="19" t="s">
         <v>15</v>
       </c>
@@ -7072,7 +7412,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="6" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A6" s="19" t="s">
         <v>15</v>
       </c>
@@ -7102,7 +7442,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" ht="15.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="19" t="s">
         <v>15</v>
       </c>
@@ -7130,7 +7470,7 @@
       <c r="I7" s="17"/>
       <c r="J7" s="10"/>
     </row>
-    <row r="8" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A8" s="19" t="s">
         <v>15</v>
       </c>
@@ -7158,7 +7498,7 @@
       </c>
       <c r="O8" s="10"/>
     </row>
-    <row r="9" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A9" s="19" t="s">
         <v>15</v>
       </c>
@@ -7186,7 +7526,7 @@
       </c>
       <c r="O9" s="10"/>
     </row>
-    <row r="10" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A10" s="19" t="s">
         <v>15</v>
       </c>
@@ -7216,7 +7556,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="11" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A11" s="19" t="s">
         <v>15</v>
       </c>
@@ -7246,7 +7586,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="12" spans="1:16" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" ht="15.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="19" t="s">
         <v>15</v>
       </c>
@@ -7274,7 +7614,7 @@
       <c r="I12" s="17"/>
       <c r="J12" s="10"/>
     </row>
-    <row r="13" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A13" s="19" t="s">
         <v>15</v>
       </c>
@@ -7302,7 +7642,7 @@
       </c>
       <c r="O13" s="10"/>
     </row>
-    <row r="14" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A14" s="19" t="s">
         <v>15</v>
       </c>
@@ -7330,7 +7670,7 @@
       </c>
       <c r="O14" s="10"/>
     </row>
-    <row r="15" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A15" s="19" t="s">
         <v>15</v>
       </c>
@@ -7360,7 +7700,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="16" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A16" s="19" t="s">
         <v>15</v>
       </c>
@@ -7390,7 +7730,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="17" spans="1:17" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" ht="15.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="19" t="s">
         <v>15</v>
       </c>
@@ -7418,7 +7758,7 @@
       <c r="I17" s="17"/>
       <c r="J17" s="10"/>
     </row>
-    <row r="18" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A18" s="19" t="s">
         <v>15</v>
       </c>
@@ -7446,7 +7786,7 @@
       </c>
       <c r="O18" s="10"/>
     </row>
-    <row r="19" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A19" s="19" t="s">
         <v>15</v>
       </c>
@@ -7474,7 +7814,7 @@
       </c>
       <c r="O19" s="10"/>
     </row>
-    <row r="20" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A20" s="19" t="s">
         <v>15</v>
       </c>
@@ -7504,7 +7844,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="21" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A21" s="19" t="s">
         <v>15</v>
       </c>
@@ -7534,7 +7874,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="22" spans="1:17" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" ht="15.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A22" s="19" t="s">
         <v>15</v>
       </c>
@@ -7562,7 +7902,7 @@
       <c r="I22" s="17"/>
       <c r="J22" s="10"/>
     </row>
-    <row r="23" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A23" s="19" t="s">
         <v>15</v>
       </c>
@@ -7590,7 +7930,7 @@
       </c>
       <c r="O23" s="10"/>
     </row>
-    <row r="24" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A24" s="19" t="s">
         <v>15</v>
       </c>
@@ -7618,7 +7958,7 @@
       </c>
       <c r="O24" s="10"/>
     </row>
-    <row r="25" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A25" s="19" t="s">
         <v>15</v>
       </c>
@@ -7648,7 +7988,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="26" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A26" s="19" t="s">
         <v>15</v>
       </c>
@@ -7678,7 +8018,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="27" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A27" s="19" t="s">
         <v>15</v>
       </c>
@@ -7713,7 +8053,7 @@
       <c r="P27" s="31"/>
       <c r="Q27" s="31"/>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A28" s="19" t="s">
         <v>15</v>
       </c>
@@ -7748,7 +8088,7 @@
       <c r="P28" s="31"/>
       <c r="Q28" s="31"/>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A29" s="19" t="s">
         <v>15</v>
       </c>
@@ -7783,7 +8123,7 @@
       <c r="P29" s="31"/>
       <c r="Q29" s="31"/>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A30" s="19" t="s">
         <v>15</v>
       </c>
@@ -7820,7 +8160,7 @@
       <c r="P30" s="31"/>
       <c r="Q30" s="31"/>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A31" s="19" t="s">
         <v>15</v>
       </c>
@@ -7857,7 +8197,7 @@
       <c r="P31" s="31"/>
       <c r="Q31" s="31"/>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A32" s="19" t="s">
         <v>15</v>
       </c>
@@ -7892,7 +8232,7 @@
       <c r="P32" s="31"/>
       <c r="Q32" s="34"/>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A33" s="19" t="s">
         <v>15</v>
       </c>
@@ -7927,7 +8267,7 @@
       <c r="P33" s="31"/>
       <c r="Q33" s="34"/>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A34" s="19" t="s">
         <v>15</v>
       </c>
@@ -7962,7 +8302,7 @@
       <c r="P34" s="31"/>
       <c r="Q34" s="34"/>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A35" s="19" t="s">
         <v>15</v>
       </c>
@@ -7999,7 +8339,7 @@
       <c r="P35" s="31"/>
       <c r="Q35" s="34"/>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A36" s="19" t="s">
         <v>15</v>
       </c>
@@ -8036,7 +8376,7 @@
       <c r="P36" s="31"/>
       <c r="Q36" s="34"/>
     </row>
-    <row r="37" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:17" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A37" s="19" t="s">
         <v>15</v>
       </c>
@@ -8071,7 +8411,7 @@
       <c r="P37" s="34"/>
       <c r="Q37" s="34"/>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A38" s="19" t="s">
         <v>15</v>
       </c>
@@ -8105,7 +8445,7 @@
       <c r="P38" s="34"/>
       <c r="Q38" s="34"/>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A39" s="19" t="s">
         <v>15</v>
       </c>
@@ -8139,7 +8479,7 @@
       <c r="P39" s="34"/>
       <c r="Q39" s="34"/>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A40" s="19" t="s">
         <v>15</v>
       </c>
@@ -8175,7 +8515,7 @@
       <c r="P40" s="31"/>
       <c r="Q40" s="31"/>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A41" s="19" t="s">
         <v>15</v>
       </c>
@@ -8211,7 +8551,7 @@
       <c r="P41" s="31"/>
       <c r="Q41" s="34"/>
     </row>
-    <row r="42" spans="1:17" s="75" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:17" s="75" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A42" s="19" t="s">
         <v>15</v>
       </c>
@@ -8236,7 +8576,7 @@
       <c r="N42" s="74"/>
       <c r="O42" s="74"/>
     </row>
-    <row r="43" spans="1:17" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:17" ht="15.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A43" s="19" t="s">
         <v>15</v>
       </c>
@@ -8264,7 +8604,7 @@
       <c r="I43" s="17"/>
       <c r="J43" s="10"/>
     </row>
-    <row r="44" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A44" s="19" t="s">
         <v>15</v>
       </c>
@@ -8292,7 +8632,7 @@
       </c>
       <c r="O44" s="10"/>
     </row>
-    <row r="45" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A45" s="19" t="s">
         <v>15</v>
       </c>
@@ -8322,7 +8662,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="46" spans="1:17" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:17" ht="15.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A46" s="19" t="s">
         <v>15</v>
       </c>
@@ -8350,7 +8690,7 @@
       <c r="I46" s="17"/>
       <c r="J46" s="10"/>
     </row>
-    <row r="47" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A47" s="19" t="s">
         <v>15</v>
       </c>
@@ -8378,7 +8718,7 @@
       </c>
       <c r="O47" s="10"/>
     </row>
-    <row r="48" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A48" s="19" t="s">
         <v>15</v>
       </c>
@@ -8408,7 +8748,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="49" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A49" s="19" t="s">
         <v>15</v>
       </c>
@@ -8438,7 +8778,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="50" spans="1:16" s="75" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:16" s="75" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A50" s="73" t="s">
         <v>15</v>
       </c>
@@ -8461,7 +8801,7 @@
       <c r="N50" s="74"/>
       <c r="O50" s="74"/>
     </row>
-    <row r="51" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A51" s="19" t="s">
         <v>15</v>
       </c>
@@ -8495,7 +8835,7 @@
       <c r="O51" s="37"/>
       <c r="P51" s="37"/>
     </row>
-    <row r="52" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A52" s="19" t="s">
         <v>15</v>
       </c>
@@ -8529,7 +8869,7 @@
       <c r="O52" s="37"/>
       <c r="P52" s="37"/>
     </row>
-    <row r="53" spans="1:16" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:16" ht="15.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A53" s="19" t="s">
         <v>15</v>
       </c>
@@ -8563,7 +8903,7 @@
       <c r="O53" s="37"/>
       <c r="P53" s="37"/>
     </row>
-    <row r="54" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A54" s="19" t="s">
         <v>15</v>
       </c>
@@ -8599,7 +8939,7 @@
       </c>
       <c r="P54" s="37"/>
     </row>
-    <row r="55" spans="1:16" s="75" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A55" s="73" t="s">
         <v>15</v>
       </c>
@@ -8622,7 +8962,7 @@
       <c r="N55" s="74"/>
       <c r="O55" s="74"/>
     </row>
-    <row r="56" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A56" s="19" t="s">
         <v>15</v>
       </c>
@@ -8656,7 +8996,7 @@
       <c r="O56" s="37"/>
       <c r="P56" s="37"/>
     </row>
-    <row r="57" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A57" s="19" t="s">
         <v>15</v>
       </c>
@@ -8690,7 +9030,7 @@
       <c r="O57" s="37"/>
       <c r="P57" s="37"/>
     </row>
-    <row r="58" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A58" s="19" t="s">
         <v>15</v>
       </c>
@@ -8724,7 +9064,7 @@
       <c r="O58" s="37"/>
       <c r="P58" s="37"/>
     </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A59" s="19" t="s">
         <v>15</v>
       </c>
@@ -8760,7 +9100,7 @@
       </c>
       <c r="P59" s="37"/>
     </row>
-    <row r="60" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:16" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A60" s="19" t="s">
         <v>15</v>
       </c>
@@ -8792,7 +9132,7 @@
       <c r="O60" s="37"/>
       <c r="P60" s="37"/>
     </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A61" s="19" t="s">
         <v>15</v>
       </c>
@@ -8824,7 +9164,7 @@
       <c r="O61" s="37"/>
       <c r="P61" s="37"/>
     </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A62" s="19" t="s">
         <v>15</v>
       </c>
@@ -8856,7 +9196,7 @@
       <c r="O62" s="37"/>
       <c r="P62" s="37"/>
     </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A63" s="19" t="s">
         <v>15</v>
       </c>
@@ -8890,7 +9230,7 @@
       </c>
       <c r="P63" s="37"/>
     </row>
-    <row r="64" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:16" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A64" s="19" t="s">
         <v>15</v>
       </c>
@@ -8930,7 +9270,7 @@
       <c r="O64" s="37"/>
       <c r="P64" s="37"/>
     </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A65" s="19" t="s">
         <v>15</v>
       </c>
@@ -8964,7 +9304,7 @@
       <c r="O65" s="37"/>
       <c r="P65" s="37"/>
     </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A66" s="19" t="s">
         <v>15</v>
       </c>
@@ -9000,7 +9340,7 @@
       </c>
       <c r="P66" s="37"/>
     </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A67" s="19" t="s">
         <v>15</v>
       </c>
@@ -9171,24 +9511,24 @@
       <selection pane="bottomLeft" activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="12" style="14" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28" customWidth="1"/>
-    <col min="3" max="3" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.5703125" customWidth="1"/>
-    <col min="5" max="5" width="60.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.86328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.59765625" customWidth="1"/>
+    <col min="5" max="5" width="60.265625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="42" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="43.140625" customWidth="1"/>
-    <col min="9" max="9" width="5.5703125" customWidth="1"/>
-    <col min="10" max="10" width="5.85546875" customWidth="1"/>
-    <col min="11" max="11" width="4.42578125" customWidth="1"/>
-    <col min="13" max="13" width="45.42578125" customWidth="1"/>
+    <col min="7" max="7" width="10.73046875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="43.1328125" customWidth="1"/>
+    <col min="9" max="9" width="5.59765625" customWidth="1"/>
+    <col min="10" max="10" width="5.86328125" customWidth="1"/>
+    <col min="11" max="11" width="4.3984375" customWidth="1"/>
+    <col min="13" max="13" width="45.3984375" customWidth="1"/>
     <col min="15" max="15" width="26" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="41" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" s="41" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="87" t="s">
         <v>0</v>
       </c>
@@ -9235,7 +9575,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15" s="79" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" s="79" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A2" s="88" t="s">
         <v>15</v>
       </c>
@@ -9257,7 +9597,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="3" spans="1:15" s="52" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" s="52" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A3" s="89" t="s">
         <v>15</v>
       </c>
@@ -9277,7 +9617,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A4" s="71" t="s">
         <v>15</v>
       </c>
@@ -9303,7 +9643,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="5" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A5" s="71" t="s">
         <v>15</v>
       </c>
@@ -9338,7 +9678,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="6" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A6" s="71" t="s">
         <v>15</v>
       </c>
@@ -9373,7 +9713,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="7" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A7" s="71" t="s">
         <v>15</v>
       </c>
@@ -9408,7 +9748,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="8" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A8" s="71" t="s">
         <v>15</v>
       </c>
@@ -9443,7 +9783,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="9" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A9" s="71" t="s">
         <v>15</v>
       </c>
@@ -9478,7 +9818,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="10" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A10" s="71" t="s">
         <v>15</v>
       </c>
@@ -9513,7 +9853,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A11" s="71" t="s">
         <v>15</v>
       </c>
@@ -9542,7 +9882,7 @@
       <c r="J11" s="12"/>
       <c r="K11" s="12"/>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A12" s="71" t="s">
         <v>15</v>
       </c>
@@ -9577,7 +9917,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A13" s="71" t="s">
         <v>15</v>
       </c>
@@ -9609,7 +9949,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A14" s="71" t="s">
         <v>15</v>
       </c>
@@ -9644,7 +9984,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A15" s="71" t="s">
         <v>15</v>
       </c>
@@ -9679,7 +10019,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A16" s="71" t="s">
         <v>15</v>
       </c>
@@ -9714,7 +10054,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A17" s="71" t="s">
         <v>15</v>
       </c>
@@ -9749,7 +10089,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A18" s="71" t="s">
         <v>15</v>
       </c>
@@ -9784,7 +10124,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="19" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A19" s="71" t="s">
         <v>15</v>
       </c>
@@ -9813,7 +10153,7 @@
       <c r="J19" s="12"/>
       <c r="K19" s="12"/>
     </row>
-    <row r="20" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A20" s="71" t="s">
         <v>15</v>
       </c>
@@ -9848,7 +10188,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="21" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A21" s="71" t="s">
         <v>15</v>
       </c>
@@ -9883,7 +10223,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="22" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A22" s="71" t="s">
         <v>15</v>
       </c>
@@ -9918,7 +10258,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="23" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A23" s="71" t="s">
         <v>15</v>
       </c>
@@ -10007,24 +10347,24 @@
       <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="12" style="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.85546875" customWidth="1"/>
-    <col min="3" max="3" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.7109375" customWidth="1"/>
+    <col min="2" max="2" width="20.86328125" customWidth="1"/>
+    <col min="3" max="3" width="6.86328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.73046875" customWidth="1"/>
     <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.85546875" customWidth="1"/>
-    <col min="7" max="7" width="7.5703125" customWidth="1"/>
-    <col min="8" max="8" width="50.5703125" customWidth="1"/>
-    <col min="9" max="9" width="5.28515625" customWidth="1"/>
-    <col min="10" max="10" width="5.7109375" customWidth="1"/>
-    <col min="11" max="11" width="4.85546875" customWidth="1"/>
+    <col min="6" max="6" width="11.86328125" customWidth="1"/>
+    <col min="7" max="7" width="7.59765625" customWidth="1"/>
+    <col min="8" max="8" width="50.59765625" customWidth="1"/>
+    <col min="9" max="9" width="5.265625" customWidth="1"/>
+    <col min="10" max="10" width="5.73046875" customWidth="1"/>
+    <col min="11" max="11" width="4.86328125" customWidth="1"/>
     <col min="13" max="13" width="34" customWidth="1"/>
-    <col min="15" max="15" width="23.5703125" customWidth="1"/>
+    <col min="15" max="15" width="23.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="48" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" s="48" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="90" t="s">
         <v>0</v>
       </c>
@@ -10071,7 +10411,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15" s="43" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" s="43" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A2" s="80" t="s">
         <v>15</v>
       </c>
@@ -10089,7 +10429,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="135" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" ht="99.75" x14ac:dyDescent="0.45">
       <c r="A3" s="14" t="s">
         <v>15</v>
       </c>
@@ -10115,7 +10455,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A4" s="14" t="s">
         <v>15</v>
       </c>
@@ -10141,7 +10481,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A5" s="14" t="s">
         <v>15</v>
       </c>
@@ -10167,7 +10507,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A6" s="14" t="s">
         <v>15</v>
       </c>
@@ -10193,7 +10533,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A7" s="14" t="s">
         <v>15</v>
       </c>
@@ -10219,7 +10559,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A8" s="14" t="s">
         <v>15</v>
       </c>
@@ -10248,7 +10588,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A9" s="14" t="s">
         <v>15</v>
       </c>
@@ -10277,7 +10617,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A10" s="14" t="s">
         <v>15</v>
       </c>
@@ -10306,7 +10646,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A11" s="14" t="s">
         <v>15</v>
       </c>
@@ -10335,7 +10675,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A12" s="14" t="s">
         <v>15</v>
       </c>
@@ -10364,7 +10704,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A13" s="14" t="s">
         <v>15</v>
       </c>
@@ -10393,7 +10733,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A14" s="14" t="s">
         <v>15</v>
       </c>
@@ -10422,7 +10762,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A15" s="14" t="s">
         <v>15</v>
       </c>
@@ -10467,6 +10807,300 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56A84AC3-0599-4EBA-84AF-FCF7BB5B65B2}">
+  <dimension ref="A1:O9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="10.19921875" customWidth="1"/>
+    <col min="2" max="2" width="33.19921875" customWidth="1"/>
+    <col min="5" max="5" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.73046875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="41.33203125" customWidth="1"/>
+    <col min="13" max="13" width="33.1328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" s="48" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="90" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="48" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="48" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="48" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="48" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="48" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="48" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="48" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="48" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="48" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="48" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="48" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="48" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="48" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" s="43" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A2" s="80" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
+        <v>521</v>
+      </c>
+      <c r="C2" s="44" t="s">
+        <v>345</v>
+      </c>
+      <c r="E2" s="43" t="s">
+        <v>346</v>
+      </c>
+      <c r="H2" s="47" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
+        <v>521</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>522</v>
+      </c>
+      <c r="D3" s="60" t="s">
+        <v>345</v>
+      </c>
+      <c r="E3" t="s">
+        <v>523</v>
+      </c>
+      <c r="F3" t="s">
+        <v>524</v>
+      </c>
+      <c r="G3" t="s">
+        <v>32</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>521</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>522</v>
+      </c>
+      <c r="D4" s="60" t="s">
+        <v>345</v>
+      </c>
+      <c r="E4" t="s">
+        <v>523</v>
+      </c>
+      <c r="H4" s="9"/>
+      <c r="L4" s="15" t="s">
+        <v>522</v>
+      </c>
+      <c r="M4" t="s">
+        <v>523</v>
+      </c>
+      <c r="N4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
+        <v>521</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>522</v>
+      </c>
+      <c r="D5" s="60" t="s">
+        <v>345</v>
+      </c>
+      <c r="E5" t="s">
+        <v>523</v>
+      </c>
+      <c r="H5" s="9"/>
+      <c r="L5" s="15" t="s">
+        <v>525</v>
+      </c>
+      <c r="M5" t="s">
+        <v>526</v>
+      </c>
+      <c r="N5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>521</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>522</v>
+      </c>
+      <c r="D6" s="60" t="s">
+        <v>345</v>
+      </c>
+      <c r="E6" t="s">
+        <v>523</v>
+      </c>
+      <c r="H6" s="9"/>
+      <c r="L6" s="15" t="s">
+        <v>527</v>
+      </c>
+      <c r="M6" t="s">
+        <v>528</v>
+      </c>
+      <c r="N6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
+        <v>521</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>522</v>
+      </c>
+      <c r="D7" s="60" t="s">
+        <v>345</v>
+      </c>
+      <c r="E7" t="s">
+        <v>523</v>
+      </c>
+      <c r="H7" s="9"/>
+      <c r="L7" s="15" t="s">
+        <v>529</v>
+      </c>
+      <c r="M7" t="s">
+        <v>530</v>
+      </c>
+      <c r="N7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" t="s">
+        <v>521</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>522</v>
+      </c>
+      <c r="D8" s="60" t="s">
+        <v>345</v>
+      </c>
+      <c r="E8" t="s">
+        <v>523</v>
+      </c>
+      <c r="H8" s="9"/>
+      <c r="L8" s="15" t="s">
+        <v>531</v>
+      </c>
+      <c r="M8" t="s">
+        <v>532</v>
+      </c>
+      <c r="N8" t="s">
+        <v>86</v>
+      </c>
+      <c r="O8" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" t="s">
+        <v>521</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>522</v>
+      </c>
+      <c r="D9" s="60" t="s">
+        <v>345</v>
+      </c>
+      <c r="E9" t="s">
+        <v>523</v>
+      </c>
+      <c r="H9" s="9"/>
+      <c r="L9" s="15" t="s">
+        <v>533</v>
+      </c>
+      <c r="M9" t="s">
+        <v>534</v>
+      </c>
+      <c r="N9" t="s">
+        <v>86</v>
+      </c>
+      <c r="O9" t="s">
+        <v>244</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="L4" r:id="rId1" xr:uid="{1F86DD57-E460-4A46-90F1-105CB7E424B8}"/>
+    <hyperlink ref="L5" r:id="rId2" xr:uid="{077735CA-590E-4D6C-AA3B-0E7789ED57E3}"/>
+    <hyperlink ref="L6" r:id="rId3" xr:uid="{8AAE1096-38A9-4C73-A000-84C8B703AE47}"/>
+    <hyperlink ref="L9" r:id="rId4" xr:uid="{66D94DEA-221A-4B6B-BFD1-D17FDA97DB4C}"/>
+    <hyperlink ref="L7" r:id="rId5" xr:uid="{81EF9F73-D0F4-49D5-97C4-E7656683C45A}"/>
+    <hyperlink ref="L8" r:id="rId6" xr:uid="{5505A793-00F8-480D-9211-3CC4CD2CD15F}"/>
+    <hyperlink ref="C3" r:id="rId7" xr:uid="{A973D1FB-56E5-4253-B7F7-BEF524C4344B}"/>
+    <hyperlink ref="C4:C9" r:id="rId8" display="C83118" xr:uid="{9D4117C3-6635-478D-8980-B0168187C1ED}"/>
+    <hyperlink ref="D3" r:id="rId9" xr:uid="{3BF645D5-56A9-46EE-B645-32DEF77D277F}"/>
+    <hyperlink ref="C2" r:id="rId10" xr:uid="{E0C5AAA2-F9E8-432D-AE09-F54BBC2C8A25}"/>
+    <hyperlink ref="D4:D9" r:id="rId11" display="C82571" xr:uid="{C30D6F92-7353-4DCE-A4B1-73846366C713}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{563E102B-33E4-478E-B166-9158413B6D66}">
   <dimension ref="A1:O31"/>
   <sheetViews>
@@ -10476,24 +11110,24 @@
       <selection pane="bottomLeft" activeCell="V14" sqref="V14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="12" style="14" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="49" customWidth="1"/>
     <col min="3" max="3" width="9" customWidth="1"/>
-    <col min="4" max="4" width="6.85546875" customWidth="1"/>
-    <col min="5" max="5" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.86328125" customWidth="1"/>
+    <col min="5" max="5" width="28.265625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="21" customWidth="1"/>
-    <col min="7" max="7" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="74.28515625" customWidth="1"/>
-    <col min="9" max="9" width="4.7109375" customWidth="1"/>
-    <col min="10" max="10" width="5.7109375" customWidth="1"/>
-    <col min="11" max="11" width="3.85546875" customWidth="1"/>
-    <col min="13" max="13" width="40.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="74.265625" customWidth="1"/>
+    <col min="9" max="9" width="4.73046875" customWidth="1"/>
+    <col min="10" max="10" width="5.73046875" customWidth="1"/>
+    <col min="11" max="11" width="3.86328125" customWidth="1"/>
+    <col min="13" max="13" width="40.265625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="52" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="48" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" s="48" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="90" t="s">
         <v>0</v>
       </c>
@@ -10540,7 +11174,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15" s="79" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" s="79" customFormat="1" ht="57" x14ac:dyDescent="0.45">
       <c r="A2" s="92" t="s">
         <v>15</v>
       </c>
@@ -10561,7 +11195,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="3" spans="1:15" s="43" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" s="43" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A3" s="80" t="s">
         <v>15</v>
       </c>
@@ -10584,7 +11218,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A4" s="14" t="s">
         <v>15</v>
       </c>
@@ -10610,7 +11244,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A5" s="14" t="s">
         <v>15</v>
       </c>
@@ -10641,7 +11275,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A6" s="14" t="s">
         <v>15</v>
       </c>
@@ -10667,7 +11301,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A7" s="14" t="s">
         <v>15</v>
       </c>
@@ -10693,7 +11327,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A8" s="14" t="s">
         <v>15</v>
       </c>
@@ -10719,7 +11353,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A9" s="14" t="s">
         <v>15</v>
       </c>
@@ -10748,7 +11382,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A10" s="14" t="s">
         <v>15</v>
       </c>
@@ -10777,7 +11411,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A11" s="14" t="s">
         <v>15</v>
       </c>
@@ -10803,7 +11437,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A12" s="14" t="s">
         <v>15</v>
       </c>
@@ -10829,7 +11463,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A13" s="14" t="s">
         <v>15</v>
       </c>
@@ -10858,7 +11492,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A14" s="14" t="s">
         <v>15</v>
       </c>
@@ -10887,7 +11521,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A15" s="14" t="s">
         <v>15</v>
       </c>
@@ -10913,7 +11547,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A16" s="14" t="s">
         <v>15</v>
       </c>
@@ -10942,7 +11576,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A17" s="14" t="s">
         <v>15</v>
       </c>
@@ -10971,62 +11605,62 @@
         <v>512</v>
       </c>
     </row>
-    <row r="18" spans="1:15" ht="28.7" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" ht="28.7" customHeight="1" x14ac:dyDescent="0.45">
       <c r="D18" s="15"/>
       <c r="F18" s="9"/>
       <c r="H18" s="9"/>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.45">
       <c r="D19" s="15"/>
       <c r="F19" s="9"/>
       <c r="H19" s="9"/>
       <c r="L19" s="15"/>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.45">
       <c r="D20" s="15"/>
       <c r="L20" s="15"/>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.45">
       <c r="D21" s="15"/>
       <c r="L21" s="15"/>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.45">
       <c r="D22" s="15"/>
       <c r="L22" s="15"/>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.45">
       <c r="D23" s="15"/>
       <c r="L23" s="15"/>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.45">
       <c r="D24" s="15"/>
       <c r="L24" s="15"/>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.45">
       <c r="D25" s="15"/>
       <c r="L25" s="15"/>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.45">
       <c r="D26" s="15"/>
       <c r="L26" s="15"/>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.45">
       <c r="D27" s="15"/>
       <c r="L27" s="15"/>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.45">
       <c r="D28" s="15"/>
       <c r="L28" s="15"/>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.45">
       <c r="D29" s="15"/>
       <c r="L29" s="15"/>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.45">
       <c r="D30" s="15"/>
       <c r="L30" s="15"/>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.45">
       <c r="D31" s="15"/>
       <c r="L31" s="15"/>
     </row>
@@ -11059,7 +11693,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB6A19DF-1E9E-470C-B3B2-0BC5237B4E15}">
   <dimension ref="A1:O7"/>
   <sheetViews>
@@ -11067,22 +11701,22 @@
       <selection activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="12" style="14" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="33" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="41.7109375" customWidth="1"/>
-    <col min="9" max="9" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="4.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="35.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.73046875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="41.73046875" customWidth="1"/>
+    <col min="9" max="9" width="6.3984375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="4.73046875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.86328125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="35.265625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.1328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="48" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" s="48" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="90" t="s">
         <v>0</v>
       </c>
@@ -11129,7 +11763,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15" s="43" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" s="43" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A2" s="80" t="s">
         <v>15</v>
       </c>
@@ -11146,7 +11780,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A3" s="14" t="s">
         <v>15</v>
       </c>
@@ -11173,7 +11807,7 @@
       </c>
       <c r="L3" s="37"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A4" s="14" t="s">
         <v>15</v>
       </c>
@@ -11202,7 +11836,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A5" s="14" t="s">
         <v>15</v>
       </c>
@@ -11231,7 +11865,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A6" s="14" t="s">
         <v>15</v>
       </c>
@@ -11260,7 +11894,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A7"/>
       <c r="L7" s="15" t="s">
         <v>319</v>
@@ -11293,33 +11927,33 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9941F7AF-6D9F-42D7-994E-A180BAE5303D}">
   <dimension ref="A1:O10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="12" style="98" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.85546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="9"/>
-    <col min="5" max="5" width="20.28515625" style="9" customWidth="1"/>
+    <col min="2" max="2" width="15.73046875" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.86328125" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.1328125" style="9"/>
+    <col min="5" max="5" width="20.265625" style="9" customWidth="1"/>
     <col min="6" max="6" width="27" style="9" customWidth="1"/>
-    <col min="7" max="7" width="10.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="39.5703125" style="9" customWidth="1"/>
-    <col min="9" max="9" width="6.7109375" style="9" customWidth="1"/>
-    <col min="10" max="10" width="7.140625" style="9" customWidth="1"/>
-    <col min="11" max="11" width="4.5703125" style="9" customWidth="1"/>
-    <col min="12" max="12" width="9.140625" style="9"/>
-    <col min="13" max="13" width="26.28515625" style="9" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="9"/>
+    <col min="7" max="7" width="10.265625" style="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="39.59765625" style="9" customWidth="1"/>
+    <col min="9" max="9" width="6.73046875" style="9" customWidth="1"/>
+    <col min="10" max="10" width="7.1328125" style="9" customWidth="1"/>
+    <col min="11" max="11" width="4.59765625" style="9" customWidth="1"/>
+    <col min="12" max="12" width="9.1328125" style="9"/>
+    <col min="13" max="13" width="26.265625" style="9" customWidth="1"/>
+    <col min="14" max="16384" width="9.1328125" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="49" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" s="49" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A1" s="94" t="s">
         <v>0</v>
       </c>
@@ -11366,7 +12000,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15" s="47" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" s="47" customFormat="1" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A2" s="95" t="s">
         <v>15</v>
       </c>
@@ -11388,7 +12022,7 @@
       </c>
       <c r="L2" s="97"/>
     </row>
-    <row r="3" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A3" s="98" t="s">
         <v>15</v>
       </c>
@@ -11415,7 +12049,7 @@
       </c>
       <c r="L3" s="38"/>
     </row>
-    <row r="4" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A4" s="98" t="s">
         <v>15</v>
       </c>
@@ -11444,7 +12078,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A5" s="98" t="s">
         <v>15</v>
       </c>
@@ -11473,7 +12107,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A6" s="98" t="s">
         <v>15</v>
       </c>
@@ -11502,7 +12136,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" ht="57" x14ac:dyDescent="0.45">
       <c r="A7" s="98" t="s">
         <v>15</v>
       </c>
@@ -11529,7 +12163,7 @@
       </c>
       <c r="L7" s="38"/>
     </row>
-    <row r="8" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A8" s="98" t="s">
         <v>15</v>
       </c>
@@ -11558,7 +12192,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A9" s="98" t="s">
         <v>15</v>
       </c>
@@ -11587,7 +12221,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A10" s="98" t="s">
         <v>15</v>
       </c>
@@ -11648,297 +12282,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DC7AE7F-1668-415E-8316-B69305094CC9}">
-  <dimension ref="A1:P9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O5" sqref="O5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="50" customWidth="1"/>
-    <col min="9" max="9" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="4.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="20" customWidth="1"/>
-    <col min="15" max="15" width="10.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:16" s="41" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="41" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="41" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="41" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="41" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="41" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="42" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="41" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="41" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="41" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="41" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="41" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="41" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="42" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" t="s">
-        <v>339</v>
-      </c>
-      <c r="C2" s="15" t="s">
-        <v>340</v>
-      </c>
-      <c r="D2" s="39"/>
-      <c r="E2" s="37" t="s">
-        <v>341</v>
-      </c>
-      <c r="F2" t="s">
-        <v>342</v>
-      </c>
-      <c r="G2" s="37" t="s">
-        <v>32</v>
-      </c>
-      <c r="H2" s="38" t="s">
-        <v>343</v>
-      </c>
-      <c r="I2" s="100"/>
-      <c r="J2" s="100"/>
-      <c r="K2" s="100"/>
-      <c r="L2" s="100"/>
-      <c r="M2" s="37"/>
-      <c r="N2" s="37"/>
-      <c r="O2" s="37"/>
-      <c r="P2" s="37"/>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" t="s">
-        <v>339</v>
-      </c>
-      <c r="C3" s="15" t="s">
-        <v>340</v>
-      </c>
-      <c r="D3" s="39"/>
-      <c r="E3" s="37" t="s">
-        <v>344</v>
-      </c>
-      <c r="G3" s="37"/>
-      <c r="H3" s="38"/>
-      <c r="I3" s="100"/>
-      <c r="J3" s="100"/>
-      <c r="K3" s="37"/>
-      <c r="L3" s="15" t="s">
-        <v>345</v>
-      </c>
-      <c r="M3" s="37" t="s">
-        <v>346</v>
-      </c>
-      <c r="N3" s="37" t="s">
-        <v>27</v>
-      </c>
-      <c r="O3" s="37"/>
-      <c r="P3" s="37"/>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" t="s">
-        <v>339</v>
-      </c>
-      <c r="C4" s="15" t="s">
-        <v>340</v>
-      </c>
-      <c r="D4" s="39"/>
-      <c r="E4" s="37" t="s">
-        <v>344</v>
-      </c>
-      <c r="G4" s="37"/>
-      <c r="H4" s="38"/>
-      <c r="I4" s="100"/>
-      <c r="J4" s="100"/>
-      <c r="K4" s="37"/>
-      <c r="L4" s="15" t="s">
-        <v>347</v>
-      </c>
-      <c r="M4" s="37" t="s">
-        <v>348</v>
-      </c>
-      <c r="N4" s="37" t="s">
-        <v>27</v>
-      </c>
-      <c r="O4" s="37" t="s">
-        <v>516</v>
-      </c>
-      <c r="P4" s="37"/>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" t="s">
-        <v>339</v>
-      </c>
-      <c r="C5" s="15" t="s">
-        <v>340</v>
-      </c>
-      <c r="D5" s="39"/>
-      <c r="E5" s="37" t="s">
-        <v>344</v>
-      </c>
-      <c r="G5" s="37"/>
-      <c r="H5" s="38"/>
-      <c r="I5" s="100"/>
-      <c r="J5" s="100"/>
-      <c r="K5" s="37"/>
-      <c r="L5" s="15" t="s">
-        <v>349</v>
-      </c>
-      <c r="M5" s="37" t="s">
-        <v>350</v>
-      </c>
-      <c r="N5" s="37" t="s">
-        <v>27</v>
-      </c>
-      <c r="O5" s="37"/>
-      <c r="P5" s="37"/>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" t="s">
-        <v>339</v>
-      </c>
-      <c r="C6" s="15" t="s">
-        <v>340</v>
-      </c>
-      <c r="D6" s="39"/>
-      <c r="E6" s="37" t="s">
-        <v>344</v>
-      </c>
-      <c r="G6" s="37"/>
-      <c r="H6" s="38"/>
-      <c r="I6" s="100"/>
-      <c r="J6" s="100"/>
-      <c r="K6" s="37"/>
-      <c r="L6" s="15" t="s">
-        <v>351</v>
-      </c>
-      <c r="M6" s="37" t="s">
-        <v>352</v>
-      </c>
-      <c r="N6" s="37" t="s">
-        <v>27</v>
-      </c>
-      <c r="O6" s="37"/>
-      <c r="P6" s="37"/>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" t="s">
-        <v>339</v>
-      </c>
-      <c r="C7" s="15" t="s">
-        <v>340</v>
-      </c>
-      <c r="D7" s="15"/>
-      <c r="E7" s="37" t="s">
-        <v>344</v>
-      </c>
-      <c r="H7" s="9"/>
-      <c r="L7" s="15" t="s">
-        <v>353</v>
-      </c>
-      <c r="M7" s="37" t="s">
-        <v>354</v>
-      </c>
-      <c r="N7" s="37" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" s="40"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="15"/>
-      <c r="H8" s="9"/>
-      <c r="L8" s="15"/>
-      <c r="M8" s="37"/>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="40"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="15"/>
-      <c r="H9" s="9"/>
-      <c r="L9" s="15"/>
-      <c r="M9" s="37"/>
-    </row>
-  </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="I5:J5"/>
-  </mergeCells>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <hyperlinks>
-    <hyperlink ref="L3" r:id="rId1" display="https://ncithesaurus.nci.nih.gov/ncitbrowser/ConceptReport.jsp?dictionary=NCI_Thesaurus&amp;ns=ncit&amp;code=C82571" xr:uid="{4F336F55-DA38-4BFA-A8FE-1B50799B12D9}"/>
-    <hyperlink ref="L4" r:id="rId2" display="https://evsexplore.nci.nih.gov/evsexplore/concept/ncit/C82977" xr:uid="{84616E4F-44BE-4656-94FE-3CAEDF7CDCB9}"/>
-    <hyperlink ref="L5" r:id="rId3" display="https://ncithesaurus.nci.nih.gov/ncitbrowser/ConceptReport.jsp?dictionary=NCI_Thesaurus&amp;ns=ncit&amp;code=C25372" xr:uid="{7D202BF9-76BC-40DB-9E31-E3CC4E640E24}"/>
-    <hyperlink ref="L6" r:id="rId4" display="https://ncithesaurus.nci.nih.gov/ncitbrowser/ConceptReport.jsp?dictionary=NCI_Thesaurus&amp;ns=ncit&amp;code=C25692" xr:uid="{089EDE5B-41FF-4CA6-878A-1C77F1E5873E}"/>
-    <hyperlink ref="C2" r:id="rId5" xr:uid="{8CA55E9B-8F6C-4EFA-BFDA-4D26710188D6}"/>
-    <hyperlink ref="C3:C6" r:id="rId6" display="C70945" xr:uid="{3EAC77A3-7633-4967-9FE5-4584FEB6951E}"/>
-    <hyperlink ref="L7" r:id="rId7" xr:uid="{3A80CB5A-691C-4326-A475-9708183012A1}"/>
-    <hyperlink ref="C7" r:id="rId8" xr:uid="{1C9D9F76-9433-40B0-AF2A-78150A167C1E}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -11948,15 +12291,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100EA3DD6FD0640724CAC6A104AA4040E53" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="95a591a9c1d64a7009b5597c446bd65f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3dc215b4-4765-4137-95ef-e24fb8216673" xmlns:ns3="2634c873-c79e-4fdd-b8bf-a33e5fa5c27f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="63634f6e381b5ed55a864cdabf38da8d" ns2:_="" ns3:_="">
     <xsd:import namespace="3dc215b4-4765-4137-95ef-e24fb8216673"/>
@@ -12181,32 +12515,33 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1C7FF019-6E9E-4327-8A98-09E2F73626E1}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="2634c873-c79e-4fdd-b8bf-a33e5fa5c27f"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="2634c873-c79e-4fdd-b8bf-a33e5fa5c27f"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="3dc215b4-4765-4137-95ef-e24fb8216673"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9663087D-43C0-4E56-A8DA-483B09F130B4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{69987298-F94B-4FAE-824D-77320F34A719}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -12223,4 +12558,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9663087D-43C0-4E56-A8DA-483B09F130B4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>